<commit_message>
SD-70021 - CCRU - KPI template update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Supermarket - REG.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Supermarket - REG.xlsx
@@ -20,6 +20,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Supermarket Regions'!$A$1:$AO$244</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Supermarket Regions'!$A$1:$AO$244</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Supermarket Regions'!$A$1:$AO$244</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Supermarket Regions'!$A$1:$AO$244</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -3029,10 +3030,10 @@
   </sheetPr>
   <dimension ref="1:245"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="Y169" activeCellId="0" sqref="Y169:Y175"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="AB181" activeCellId="0" sqref="AB181:AB184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3041,38 +3042,38 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="56.4534412955466"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="50.1336032388664"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="69.412955465587"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="56.8785425101215"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="50.5587044534413"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="70.0566801619433"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="50.2388663967611"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="2" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="3" width="9"/>
     <col collapsed="false" hidden="false" max="13" min="12" style="3" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="45.5263157894737"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="45.9554655870445"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="2" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="2" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="2" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="2" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="85.587044534413"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="55.2753036437247"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="2" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="2" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="86.336032388664"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="55.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="2" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="2" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="2" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="26.7813765182186"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="2" width="64.0566801619433"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="2" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="2" width="64.7004048582996"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="2" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="2" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="39" min="39" style="2" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="2" width="10.6032388663968"/>
@@ -18110,8 +18111,8 @@
       <c r="Y181" s="10"/>
       <c r="Z181" s="10"/>
       <c r="AA181" s="10"/>
-      <c r="AB181" s="10" t="n">
-        <v>1103</v>
+      <c r="AB181" s="20" t="n">
+        <v>1102</v>
       </c>
       <c r="AC181" s="10"/>
       <c r="AD181" s="10"/>
@@ -18198,8 +18199,8 @@
       <c r="Y182" s="10"/>
       <c r="Z182" s="10"/>
       <c r="AA182" s="10"/>
-      <c r="AB182" s="10" t="n">
-        <v>1103</v>
+      <c r="AB182" s="20" t="n">
+        <v>1102</v>
       </c>
       <c r="AC182" s="10"/>
       <c r="AD182" s="10"/>
@@ -18278,8 +18279,8 @@
       <c r="Y183" s="10"/>
       <c r="Z183" s="10"/>
       <c r="AA183" s="10"/>
-      <c r="AB183" s="10" t="n">
-        <v>1103</v>
+      <c r="AB183" s="20" t="n">
+        <v>1102</v>
       </c>
       <c r="AC183" s="10"/>
       <c r="AD183" s="10"/>
@@ -18360,8 +18361,8 @@
       <c r="Y184" s="10"/>
       <c r="Z184" s="10"/>
       <c r="AA184" s="10"/>
-      <c r="AB184" s="10" t="n">
-        <v>1103</v>
+      <c r="AB184" s="20" t="n">
+        <v>1102</v>
       </c>
       <c r="AC184" s="10"/>
       <c r="AD184" s="10"/>

</xml_diff>